<commit_message>
double check create invoice
</commit_message>
<xml_diff>
--- a/aceess/thang8.xlsx
+++ b/aceess/thang8.xlsx
@@ -26797,9 +26797,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K979"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -33918,7 +33918,7 @@
   <dimension ref="A2:AB105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>